<commit_message>
Fix error in Device mapping
</commit_message>
<xml_diff>
--- a/maps/Device-and-DeviceUse.xlsx
+++ b/maps/Device-and-DeviceUse.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\mgraauw\eu-nl-compared\maps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edelman_nict1\eu-nl-compared\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C5DADA2-EDCF-4712-B932-3BEA73B38E5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2A08A29E-9454-4354-9B9A-663A1D942DE6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7005" yWindow="2235" windowWidth="21600" windowHeight="12735" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -498,8 +498,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -566,9 +566,6 @@
       <c r="A10" t="s">
         <v>8</v>
       </c>
-      <c r="B10" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -578,6 +575,9 @@
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
+      </c>
+      <c r="B12" t="s">
+        <v>15</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Add mappings for HealthProfessional, BodyStructure, Location and Organization
</commit_message>
<xml_diff>
--- a/maps/Device-and-DeviceUse.xlsx
+++ b/maps/Device-and-DeviceUse.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edelman_nict1\eu-nl-compared\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36E93E42-7F6F-415D-A09A-96F7FCDB30D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F49294-D114-46CB-B045-3A5FD2A26664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>EHDSDevice</t>
   </si>
@@ -74,9 +74,6 @@
   </si>
   <si>
     <t>zib</t>
-  </si>
-  <si>
-    <t>MedicalDevice.Indication::Problem</t>
   </si>
   <si>
     <t>MedicalDevice.ProductDescription</t>
@@ -499,10 +496,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B29"/>
+  <dimension ref="A1:B28"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -590,7 +587,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
         <v>12</v>
@@ -598,77 +595,74 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B22" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>38</v>
-      </c>
-      <c r="B26" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -677,16 +671,11 @@
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>37</v>
+      </c>
       <c r="B28" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>38</v>
-      </c>
-      <c r="B29" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated XtEHR Device and DeviceUse
</commit_message>
<xml_diff>
--- a/maps/Device-and-DeviceUse.xlsx
+++ b/maps/Device-and-DeviceUse.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edelman_nict1\eu-nl-compared\maps\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Nictiz\eu-nl-compared\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5F49294-D114-46CB-B045-3A5FD2A26664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901EF396-F93E-4DFD-A979-E02C0294E734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-13500" yWindow="-21600" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
   <si>
     <t>EHDSDevice</t>
   </si>
@@ -97,24 +97,12 @@
     <t>EHDSDeviceUse</t>
   </si>
   <si>
-    <t>EHDSDeviceUse.identifier</t>
-  </si>
-  <si>
     <t>EHDSDeviceUse.status</t>
   </si>
   <si>
-    <t>EHDSDeviceUse.implantDate</t>
-  </si>
-  <si>
     <t>EHDSDeviceUse.endDate</t>
   </si>
   <si>
-    <t>EHDSDeviceUse.device</t>
-  </si>
-  <si>
-    <t>EHDSDeviceUse.subject</t>
-  </si>
-  <si>
     <t>EHDSDeviceUse.bodySite</t>
   </si>
   <si>
@@ -124,16 +112,58 @@
     <t>EHDSDeviceUse.recorded</t>
   </si>
   <si>
-    <t>EHDSDeviceUse.source</t>
-  </si>
-  <si>
     <t>MedicalDevice.EndDate</t>
   </si>
   <si>
     <t>MedicalDevice.Indication::Diagnosis</t>
   </si>
   <si>
-    <t>EHDSDeviceUse.reason</t>
+    <t>EHDSDeviceUse.header</t>
+  </si>
+  <si>
+    <t>EHDSDeviceUse.header.subject</t>
+  </si>
+  <si>
+    <t>EHDSDeviceUse.header.identifier</t>
+  </si>
+  <si>
+    <t>EHDSDeviceUse.header.authorship</t>
+  </si>
+  <si>
+    <t>EHDSDeviceUse.header.authorship.author[x]</t>
+  </si>
+  <si>
+    <t>EHDSDeviceUse.header.authorship.datetime</t>
+  </si>
+  <si>
+    <t>EHDSDeviceUse.header.lastUpdate</t>
+  </si>
+  <si>
+    <t>EHDSDeviceUse.header.status</t>
+  </si>
+  <si>
+    <t>EHDSDeviceUse.header.statusReason[x]</t>
+  </si>
+  <si>
+    <t>EHDSDeviceUse.header.language</t>
+  </si>
+  <si>
+    <t>EHDSDeviceUse.header.version</t>
+  </si>
+  <si>
+    <t>EHDSDeviceUse.presentedForm</t>
+  </si>
+  <si>
+    <t>EHDSDeviceUse.startDate</t>
+  </si>
+  <si>
+    <t>EHDSDeviceUse.device[x]</t>
+  </si>
+  <si>
+    <t>EHDSDeviceUse.reason[x]</t>
+  </si>
+  <si>
+    <t>EHDSDeviceUse.source[x]</t>
   </si>
 </sst>
 </file>
@@ -496,10 +526,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B28"/>
+  <dimension ref="A1:B38"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B33" sqref="B33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -595,90 +625,141 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>25</v>
+        <v>32</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>27</v>
-      </c>
-      <c r="B17" t="s">
-        <v>23</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>28</v>
-      </c>
-      <c r="B18" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>31</v>
-      </c>
-      <c r="B21" t="s">
-        <v>21</v>
+        <v>38</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>32</v>
-      </c>
-      <c r="B22" t="s">
-        <v>22</v>
+        <v>39</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>34</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B25" t="s">
-        <v>18</v>
+      <c r="A25" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>19</v>
+      <c r="A26" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B27" t="s">
-        <v>20</v>
+      <c r="A27" t="s">
+        <v>25</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
       <c r="B28" t="s">
-        <v>36</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>26</v>
+      </c>
+      <c r="B29" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>27</v>
+      </c>
+      <c r="B31" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>28</v>
+      </c>
+      <c r="B32" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B36" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B37" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>46</v>
+      </c>
+      <c r="B38" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Comments file with changes as of 16-7
</commit_message>
<xml_diff>
--- a/maps/Device-and-DeviceUse.xlsx
+++ b/maps/Device-and-DeviceUse.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Source\Nictiz\eu-nl-compared\maps\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{901EF396-F93E-4DFD-A979-E02C0294E734}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FE07AA51-6D2A-4A6C-9264-386B0094582C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-13500" yWindow="-21600" windowWidth="26010" windowHeight="20985" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,12 +20,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>EHDSDevice</t>
-  </si>
-  <si>
-    <t>EHDSDevice.identifier</t>
   </si>
   <si>
     <t>EHDSDevice.manufacturer</t>
@@ -526,10 +523,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B38"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+      <selection activeCell="A27" sqref="A27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -540,10 +537,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -551,16 +548,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>1</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
@@ -601,26 +595,26 @@
       <c r="A11" t="s">
         <v>9</v>
       </c>
+      <c r="B11" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>10</v>
       </c>
-      <c r="B12" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="B13" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>24</v>
-      </c>
-      <c r="B14" t="s">
-        <v>12</v>
+        <v>31</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
@@ -632,6 +626,9 @@
       <c r="A16" t="s">
         <v>33</v>
       </c>
+      <c r="B16" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
@@ -680,33 +677,36 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>43</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>43</v>
+      </c>
+      <c r="B27" t="s">
+        <v>22</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>44</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" t="s">
-        <v>30</v>
+        <v>44</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>45</v>
+        <v>26</v>
+      </c>
+      <c r="B30" t="s">
+        <v>20</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -721,18 +721,15 @@
       <c r="A32" t="s">
         <v>28</v>
       </c>
-      <c r="B32" t="s">
-        <v>22</v>
-      </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>29</v>
+        <v>46</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>47</v>
+      <c r="B34" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
@@ -746,16 +743,11 @@
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>45</v>
+      </c>
       <c r="B37" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>46</v>
-      </c>
-      <c r="B38" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>